<commit_message>
Adjust poster for readability
</commit_message>
<xml_diff>
--- a/testresults.xlsx
+++ b/testresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramj\Documents\Ingenieur\WIT\MASTER_2\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177D75C7-7EA0-431C-BE8D-504CB03DECA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB59E2BF-A37F-4CFC-B230-1CCD9B87C905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{2A192508-2A1C-480C-94C6-ADC644D4972E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A192508-2A1C-480C-94C6-ADC644D4972E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -691,10 +691,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="104"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="4"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -705,7 +705,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="95000"/>
@@ -724,7 +724,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Temporal refinement</a:t>
             </a:r>
           </a:p>
@@ -743,7 +743,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="95000"/>
@@ -777,7 +777,7 @@
           <c:spPr>
             <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -796,21 +796,21 @@
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="0">
-                    <a:schemeClr val="accent1">
+                    <a:schemeClr val="accent2">
                       <a:satMod val="103000"/>
                       <a:lumMod val="102000"/>
                       <a:tint val="94000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
+                    <a:schemeClr val="accent2">
                       <a:satMod val="110000"/>
                       <a:lumMod val="100000"/>
                       <a:shade val="100000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
+                    <a:schemeClr val="accent2">
                       <a:lumMod val="99000"/>
                       <a:satMod val="120000"/>
                       <a:shade val="78000"/>
@@ -821,7 +821,7 @@
               </a:gradFill>
               <a:ln w="9525" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -940,15 +940,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Δt_c/</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="el-GR"/>
+                  <a:rPr lang="el-GR" sz="1800"/>
                   <a:t>Δ</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>t_F</a:t>
                 </a:r>
               </a:p>
@@ -1002,7 +1002,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
@@ -1060,7 +1060,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>speedup</a:t>
                 </a:r>
               </a:p>
@@ -1114,7 +1114,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
@@ -4100,42 +4100,8 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="22">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -7888,8 +7854,8 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8417,8 +8383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C33A822-2F37-4EAE-9049-0190C56A678D}">
   <dimension ref="A2:U87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="U48" sqref="U48"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>